<commit_message>
xcel added for signup
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Scripts for Testing\maven-testng\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE50CDE0-E959-4C94-A6BA-448EA8CC042C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50792C2F-A381-4D2E-B783-56A179A61463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="createUnderWriterSheet" sheetId="2" r:id="rId2"/>
+    <sheet name="userLoginSheet" sheetId="3" r:id="rId3"/>
+    <sheet name="createAdminSheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="172">
   <si>
     <t xml:space="preserve">shivam </t>
   </si>
@@ -154,13 +157,400 @@
   </si>
   <si>
     <t>ppppp@ppp.com</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>writerId</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>sdfsdfgs</t>
+  </si>
+  <si>
+    <t>UW12</t>
+  </si>
+  <si>
+    <t>dscds123</t>
+  </si>
+  <si>
+    <t>dscds124</t>
+  </si>
+  <si>
+    <t>dscds125</t>
+  </si>
+  <si>
+    <t>dscds126</t>
+  </si>
+  <si>
+    <t>dscds127</t>
+  </si>
+  <si>
+    <t>dscds128</t>
+  </si>
+  <si>
+    <t>dscds129</t>
+  </si>
+  <si>
+    <t>dscds130</t>
+  </si>
+  <si>
+    <t>dscds131</t>
+  </si>
+  <si>
+    <t>dscds132</t>
+  </si>
+  <si>
+    <t>dscds133</t>
+  </si>
+  <si>
+    <t>dscds134</t>
+  </si>
+  <si>
+    <t>dscds135</t>
+  </si>
+  <si>
+    <t>dscds136</t>
+  </si>
+  <si>
+    <t>dscds137</t>
+  </si>
+  <si>
+    <t>dscds138</t>
+  </si>
+  <si>
+    <t>dscds139</t>
+  </si>
+  <si>
+    <t>dscds140</t>
+  </si>
+  <si>
+    <t>dscds141</t>
+  </si>
+  <si>
+    <t>dscds142</t>
+  </si>
+  <si>
+    <t>UW13</t>
+  </si>
+  <si>
+    <t>UW14</t>
+  </si>
+  <si>
+    <t>UW15</t>
+  </si>
+  <si>
+    <t>UW16</t>
+  </si>
+  <si>
+    <t>UW17</t>
+  </si>
+  <si>
+    <t>UW18</t>
+  </si>
+  <si>
+    <t>UW19</t>
+  </si>
+  <si>
+    <t>UW20</t>
+  </si>
+  <si>
+    <t>UW21</t>
+  </si>
+  <si>
+    <t>UW22</t>
+  </si>
+  <si>
+    <t>UW23</t>
+  </si>
+  <si>
+    <t>UW24</t>
+  </si>
+  <si>
+    <t>UW25</t>
+  </si>
+  <si>
+    <t>UW26</t>
+  </si>
+  <si>
+    <t>UW27</t>
+  </si>
+  <si>
+    <t>UW28</t>
+  </si>
+  <si>
+    <t>UW29</t>
+  </si>
+  <si>
+    <t>UW30</t>
+  </si>
+  <si>
+    <t>UW31</t>
+  </si>
+  <si>
+    <t>nilesh</t>
+  </si>
+  <si>
+    <t>nilesh1</t>
+  </si>
+  <si>
+    <t>nilesh2</t>
+  </si>
+  <si>
+    <t>nfdg@fsd.com</t>
+  </si>
+  <si>
+    <t>shivamkumar9555@gmail.com</t>
+  </si>
+  <si>
+    <t>A112345678</t>
+  </si>
+  <si>
+    <t>AdminId</t>
+  </si>
+  <si>
+    <t>ambikesh</t>
+  </si>
+  <si>
+    <t>ambikeshhitler9@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin1</t>
+  </si>
+  <si>
+    <t>sdas123456</t>
+  </si>
+  <si>
+    <t>sdas123457</t>
+  </si>
+  <si>
+    <t>sdas123458</t>
+  </si>
+  <si>
+    <t>sdas123459</t>
+  </si>
+  <si>
+    <t>sdas123460</t>
+  </si>
+  <si>
+    <t>sdas123461</t>
+  </si>
+  <si>
+    <t>sdas123462</t>
+  </si>
+  <si>
+    <t>sdas123463</t>
+  </si>
+  <si>
+    <t>sdas123464</t>
+  </si>
+  <si>
+    <t>sdas123465</t>
+  </si>
+  <si>
+    <t>sdas123466</t>
+  </si>
+  <si>
+    <t>sdas123467</t>
+  </si>
+  <si>
+    <t>sdas123468</t>
+  </si>
+  <si>
+    <t>sdas123469</t>
+  </si>
+  <si>
+    <t>sdas123470</t>
+  </si>
+  <si>
+    <t>sdas123471</t>
+  </si>
+  <si>
+    <t>sdas123472</t>
+  </si>
+  <si>
+    <t>sdas123473</t>
+  </si>
+  <si>
+    <t>sdas123474</t>
+  </si>
+  <si>
+    <t>Admin2</t>
+  </si>
+  <si>
+    <t>Admin3</t>
+  </si>
+  <si>
+    <t>Admin4</t>
+  </si>
+  <si>
+    <t>Admin5</t>
+  </si>
+  <si>
+    <t>Admin6</t>
+  </si>
+  <si>
+    <t>Admin7</t>
+  </si>
+  <si>
+    <t>Admin8</t>
+  </si>
+  <si>
+    <t>Admin9</t>
+  </si>
+  <si>
+    <t>Admin10</t>
+  </si>
+  <si>
+    <t>Admin11</t>
+  </si>
+  <si>
+    <t>Admin12</t>
+  </si>
+  <si>
+    <t>Admin13</t>
+  </si>
+  <si>
+    <t>Admin14</t>
+  </si>
+  <si>
+    <t>Admin15</t>
+  </si>
+  <si>
+    <t>Admin16</t>
+  </si>
+  <si>
+    <t>Admin17</t>
+  </si>
+  <si>
+    <t>Admin18</t>
+  </si>
+  <si>
+    <t>Admin19</t>
+  </si>
+  <si>
+    <t>ambikesh1</t>
+  </si>
+  <si>
+    <t>ambikeshhitler1@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler2@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler3@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler4@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler5@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler6@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler7@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler8@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler10@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler11@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler12@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler13@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler14@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler15@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler16@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler17@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler18@gmail.com</t>
+  </si>
+  <si>
+    <t>ambikeshhitler19@gmail.com</t>
+  </si>
+  <si>
+    <t>sdgsdg11@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg122@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg13@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg14@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg15@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg16@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg17@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg18@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg19@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg20@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg21@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg22@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg23@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg24@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg25@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg26@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg27@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdgsdg28@sdfs.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +562,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -482,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,9 +986,7 @@
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -788,6 +1182,20 @@
       </c>
       <c r="D21" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -797,26 +1205,909 @@
     <hyperlink ref="C3" r:id="rId3" xr:uid="{5D582B9D-703D-4B9B-A0FD-635338541F92}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{28F54B58-3B3C-4E29-9C28-CD8518249D78}"/>
     <hyperlink ref="C5:C16" r:id="rId5" display="sdfsf@sdfsg.com" xr:uid="{2286C9E7-4E8F-4B5B-8E82-2D9395FE000F}"/>
-    <hyperlink ref="D7" r:id="rId6" display="sfddsgs@" xr:uid="{2076E368-76E9-4277-A850-10C032DAC427}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{956C778D-F7DD-4AD2-9F3A-8E21AA6EDCFC}"/>
-    <hyperlink ref="C6" r:id="rId8" xr:uid="{7FA18995-56B2-4CE9-ACEC-C917D2D30DDB}"/>
-    <hyperlink ref="C7" r:id="rId9" xr:uid="{4EE99F4C-5DD0-4734-A01B-4D1659EF225C}"/>
-    <hyperlink ref="C8" r:id="rId10" xr:uid="{89C3755F-7AB7-447A-AEA5-9DAAA5BBCBF9}"/>
-    <hyperlink ref="C9" r:id="rId11" xr:uid="{4A0C3F81-CC1F-4F36-8D7C-FEDEFF022ADA}"/>
-    <hyperlink ref="C10" r:id="rId12" xr:uid="{C39C3282-46DE-4B80-9265-558A7818C1EA}"/>
-    <hyperlink ref="C11" r:id="rId13" xr:uid="{FD01D7B3-678E-4B91-A997-954DB8575B48}"/>
-    <hyperlink ref="C12" r:id="rId14" xr:uid="{1ECBE6E4-EEA7-4A82-B712-8EC61566F097}"/>
-    <hyperlink ref="C13" r:id="rId15" xr:uid="{5AF9988B-E79E-491A-A242-482B39621D50}"/>
-    <hyperlink ref="C14" r:id="rId16" xr:uid="{57C50869-3736-4824-8331-62BA6083EA85}"/>
-    <hyperlink ref="C15" r:id="rId17" xr:uid="{F4797CFF-55BE-4590-A5D2-8DCE37534960}"/>
-    <hyperlink ref="C16" r:id="rId18" xr:uid="{1AAD59A6-5EFB-4EE1-859B-CD74E916F45B}"/>
-    <hyperlink ref="C17" r:id="rId19" xr:uid="{E55D8C2C-1B59-4D4E-8382-F6E24E36A9BE}"/>
-    <hyperlink ref="C18:C21" r:id="rId20" display="uttamkumarsingh@gmail.com" xr:uid="{B8E64D4F-53DA-426A-B6B3-649DEB8ED7CC}"/>
-    <hyperlink ref="C18" r:id="rId21" xr:uid="{B483E33E-D31F-436E-A6EA-134A72F46DA7}"/>
-    <hyperlink ref="C19" r:id="rId22" xr:uid="{4B10FBF8-DABB-49D8-819A-9CFFA16C512F}"/>
-    <hyperlink ref="C20" r:id="rId23" xr:uid="{44FD0A7B-1AB2-4B9D-80C6-D2449BBAF32D}"/>
-    <hyperlink ref="C21" r:id="rId24" xr:uid="{ABF9DFC1-FDD1-426C-A595-D690BE24B855}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{956C778D-F7DD-4AD2-9F3A-8E21AA6EDCFC}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{7FA18995-56B2-4CE9-ACEC-C917D2D30DDB}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{4EE99F4C-5DD0-4734-A01B-4D1659EF225C}"/>
+    <hyperlink ref="C8" r:id="rId9" xr:uid="{89C3755F-7AB7-447A-AEA5-9DAAA5BBCBF9}"/>
+    <hyperlink ref="C9" r:id="rId10" xr:uid="{4A0C3F81-CC1F-4F36-8D7C-FEDEFF022ADA}"/>
+    <hyperlink ref="C10" r:id="rId11" xr:uid="{C39C3282-46DE-4B80-9265-558A7818C1EA}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{FD01D7B3-678E-4B91-A997-954DB8575B48}"/>
+    <hyperlink ref="C12" r:id="rId13" xr:uid="{1ECBE6E4-EEA7-4A82-B712-8EC61566F097}"/>
+    <hyperlink ref="C13" r:id="rId14" xr:uid="{5AF9988B-E79E-491A-A242-482B39621D50}"/>
+    <hyperlink ref="C14" r:id="rId15" xr:uid="{57C50869-3736-4824-8331-62BA6083EA85}"/>
+    <hyperlink ref="C15" r:id="rId16" xr:uid="{F4797CFF-55BE-4590-A5D2-8DCE37534960}"/>
+    <hyperlink ref="C16" r:id="rId17" xr:uid="{1AAD59A6-5EFB-4EE1-859B-CD74E916F45B}"/>
+    <hyperlink ref="C17" r:id="rId18" xr:uid="{E55D8C2C-1B59-4D4E-8382-F6E24E36A9BE}"/>
+    <hyperlink ref="C18:C21" r:id="rId19" display="uttamkumarsingh@gmail.com" xr:uid="{B8E64D4F-53DA-426A-B6B3-649DEB8ED7CC}"/>
+    <hyperlink ref="C18" r:id="rId20" xr:uid="{B483E33E-D31F-436E-A6EA-134A72F46DA7}"/>
+    <hyperlink ref="C19" r:id="rId21" xr:uid="{4B10FBF8-DABB-49D8-819A-9CFFA16C512F}"/>
+    <hyperlink ref="C20" r:id="rId22" xr:uid="{44FD0A7B-1AB2-4B9D-80C6-D2449BBAF32D}"/>
+    <hyperlink ref="C21" r:id="rId23" xr:uid="{ABF9DFC1-FDD1-426C-A595-D690BE24B855}"/>
+    <hyperlink ref="C22" r:id="rId24" xr:uid="{42279FB4-4D6C-4BA4-8020-115869F10136}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4973ED3-E61C-42D5-8CE6-08AD080CDC15}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{EC05753F-FE94-4927-9DB7-10585008DC02}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{31DC19B5-7C5C-43F9-ABB1-92E11E055F29}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{3F406CCA-DE58-41E3-BFBD-D92467B62273}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{148DA2B8-9DA5-4116-8A7A-73DBFDDF7707}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{7D3B08B7-95EE-4AB4-9828-6FE63C4B2901}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{E88D3398-B6E6-4845-9FD6-F8FF9957FD6B}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{A8859714-6683-404F-8B3E-C22B934A0402}"/>
+    <hyperlink ref="B9:B21" r:id="rId8" display="sdgsdg16@sdfs.com" xr:uid="{20AB0FA0-2FCF-4946-805C-1786454A6D88}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{63DE5FC5-7796-4B4B-81DD-D968321D9C6B}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{F913C886-98A3-41E6-BC5F-8B084A682B37}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{DB2A5EBF-0D1B-48AD-A028-6875EB1EC24C}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{AB0A9AB9-08C8-487E-BED6-CDA02C3BDD30}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{0FB8CA00-5952-4E8C-8530-1B6409D59E58}"/>
+    <hyperlink ref="B14" r:id="rId14" xr:uid="{87AD1E5E-C3C8-42BE-8BFF-D9C37FB3BB49}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{F16A30EB-5832-4AEB-8C48-00D882BCA876}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{C775F62E-B4EF-4092-A98E-62299259C923}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{5D33633F-C834-461B-A633-5E70164F146F}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{CDE686AB-472F-40A3-A751-F3DE31BC1925}"/>
+    <hyperlink ref="B19" r:id="rId19" xr:uid="{6BE61DC1-AE4E-4A8F-8B8F-2E08F8452C9C}"/>
+    <hyperlink ref="B20" r:id="rId20" xr:uid="{2CC438B5-3777-4FF2-9FC6-B490BF887D25}"/>
+    <hyperlink ref="B21" r:id="rId21" xr:uid="{D95EC583-2414-4D23-8E3A-00730D40F27E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A505EBCF-EC70-40E4-9280-A9DC40CD467D}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="sdvsdv@sdfds.com" xr:uid="{AE21C4A1-0D6A-42AA-AB47-F39A1563B09A}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{F9B166A4-D17E-41B4-80E1-8C904980A8E9}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{D2E2AC76-71ED-463A-A000-C23BFA3FB4F7}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{18BA8283-2C9A-41D7-AD75-A4E0B9CCC13A}"/>
+    <hyperlink ref="A5:A16" r:id="rId5" display="sdfsf@sdfsg.com" xr:uid="{3690F740-10EA-4B42-A020-9A3905A644E1}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{2522EB64-22D0-407B-8678-E00C02455C0A}"/>
+    <hyperlink ref="A6" r:id="rId7" xr:uid="{A2C956FD-4EE7-4D77-8E5D-2B5603032D55}"/>
+    <hyperlink ref="A7" r:id="rId8" xr:uid="{3751EE39-4977-4B5C-B762-CF0000228E79}"/>
+    <hyperlink ref="A8" r:id="rId9" xr:uid="{FA8BB3F0-FD85-4E19-B11B-E9A79110A50C}"/>
+    <hyperlink ref="A9" r:id="rId10" xr:uid="{FBE77F16-0349-483A-9972-11E7C554DE25}"/>
+    <hyperlink ref="A10" r:id="rId11" xr:uid="{B65D18DD-BE93-4931-BADA-CCA90EEB2697}"/>
+    <hyperlink ref="A11" r:id="rId12" xr:uid="{CB9EABA9-4870-4230-B5AA-E906984DB5D4}"/>
+    <hyperlink ref="A12" r:id="rId13" xr:uid="{8657B739-0D91-4540-8B8D-BF11F412F540}"/>
+    <hyperlink ref="A13" r:id="rId14" xr:uid="{05E344BB-A432-4AB3-AFAA-ED437F30F51B}"/>
+    <hyperlink ref="A14" r:id="rId15" xr:uid="{7F73881A-B13C-447F-9DCD-DA108473AC51}"/>
+    <hyperlink ref="A15" r:id="rId16" xr:uid="{99E24070-9577-4930-B517-8E836CEA4D16}"/>
+    <hyperlink ref="A16" r:id="rId17" xr:uid="{8ECB3486-22AD-4F07-B8E8-3D4B8DFF3448}"/>
+    <hyperlink ref="A17" r:id="rId18" xr:uid="{5DA32E06-6727-4DC2-AB7D-8DEB98A41C75}"/>
+    <hyperlink ref="A18:A21" r:id="rId19" display="uttamkumarsingh@gmail.com" xr:uid="{B823CACD-9B00-446B-96BC-29DB69268385}"/>
+    <hyperlink ref="A18" r:id="rId20" xr:uid="{73B8A364-A5F9-4F72-8FF2-F6C972C9A659}"/>
+    <hyperlink ref="A19" r:id="rId21" xr:uid="{0438498B-BBB2-47FA-A913-54145C32E4F1}"/>
+    <hyperlink ref="A20" r:id="rId22" xr:uid="{85C74752-ECCA-4ED1-9E29-2FBD1EB3BB44}"/>
+    <hyperlink ref="A21" r:id="rId23" xr:uid="{2468BC72-CF26-457D-BB61-3D4FBA0179BF}"/>
+    <hyperlink ref="A22" r:id="rId24" xr:uid="{A910377D-AF0A-4F65-B7CA-D280D5C14180}"/>
+    <hyperlink ref="B7" r:id="rId25" display="sfddsgs@" xr:uid="{BAA416F7-68DF-452A-8ADA-55DA2061698C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65954F3C-4D75-4AB4-A83A-42172BC3382B}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{2773C91B-515F-41D5-A3FE-B0749855A466}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{A72FB7DE-51AA-46B6-A998-F205121F52A3}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{5F8CBB91-7F97-4C85-8EDE-8C3A361EE08E}"/>
+    <hyperlink ref="B3:B20" r:id="rId4" display="ambikeshhitler9@gmail.com" xr:uid="{8874A9CC-9766-4755-82F4-0E8ABAE09A6F}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{9AE46038-BAEB-40F4-963B-946850163C67}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{471A6E2B-E858-437E-BF7D-BB70769CD52F}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{A22EDF8B-B4E5-474B-AD89-6BD19D8C3ACB}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{FA414229-7B62-4CBC-BE23-C3FAEA778D69}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{8349C84B-A7DD-44CD-8EE5-D70EE7DC439B}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{D48E1A91-906E-4C76-AFE3-C4D5A89662C1}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{BF0DFA9F-D09B-4EE2-A189-071E65D0808D}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{DD641B68-0548-4458-9BB3-4E4676782F35}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{A52536E5-33FA-4FDD-AE54-96E99698E5A1}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{14A4BB96-05C8-4A2C-9D56-54CCF3F0A14F}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{6308EA41-FEEE-45AB-9804-CE5759916A71}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{298D17A4-86AB-44E5-B766-2EBD1B335DDC}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{17A615B4-312A-4D34-9EB3-0EBBDEF769F5}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{A7D0F3B7-3329-4808-99B0-08B216EE7849}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{56C5A947-AF7D-4844-82A2-9E2D9CC18379}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
user login, signup,admin creation and uw creation test with excel and extend reports
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Scripts for Testing\maven-testng\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50792C2F-A381-4D2E-B783-56A179A61463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A52C5E-3D46-4864-BB2D-048831D9E482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="createUnderWriterSheet" sheetId="2" r:id="rId2"/>
-    <sheet name="userLoginSheet" sheetId="3" r:id="rId3"/>
-    <sheet name="createAdminSheet" sheetId="4" r:id="rId4"/>
+    <sheet name="userLoginSheet" sheetId="3" r:id="rId2"/>
+    <sheet name="createAdminSheet" sheetId="4" r:id="rId3"/>
+    <sheet name="createUnderWriterSheet" sheetId="2" r:id="rId4"/>
+    <sheet name="lifeFormData" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="207">
   <si>
     <t xml:space="preserve">shivam </t>
   </si>
@@ -544,6 +545,111 @@
   </si>
   <si>
     <t>sdgsdg28@sdfs.com</t>
+  </si>
+  <si>
+    <t>sdfdsf</t>
+  </si>
+  <si>
+    <t>fsd</t>
+  </si>
+  <si>
+    <t>fsdf</t>
+  </si>
+  <si>
+    <t>sdfsdfsd</t>
+  </si>
+  <si>
+    <t>ssdfsdf</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>aadhar</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>selectplane</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>healthIssue</t>
+  </si>
+  <si>
+    <t>cancellingInsurance</t>
+  </si>
+  <si>
+    <t>groupInsurance</t>
+  </si>
+  <si>
+    <t>tobacco</t>
+  </si>
+  <si>
+    <t>hivIssue</t>
+  </si>
+  <si>
+    <t>lungsIssue</t>
+  </si>
+  <si>
+    <t>additionalComments</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>2 Years</t>
+  </si>
+  <si>
+    <t>5lacs</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Agra</t>
   </si>
 </sst>
 </file>
@@ -594,9 +700,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -880,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,6 +1306,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" display="sdvsdv@sdfds.com" xr:uid="{EE755B02-7380-4A9B-B5EE-CB261AF69109}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{28FC4BFD-C9B9-4A35-9B96-DE41AF25005A}"/>
@@ -1230,349 +1338,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4973ED3-E61C-42D5-8CE6-08AD080CDC15}">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{EC05753F-FE94-4927-9DB7-10585008DC02}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{31DC19B5-7C5C-43F9-ABB1-92E11E055F29}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{3F406CCA-DE58-41E3-BFBD-D92467B62273}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{148DA2B8-9DA5-4116-8A7A-73DBFDDF7707}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{7D3B08B7-95EE-4AB4-9828-6FE63C4B2901}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{E88D3398-B6E6-4845-9FD6-F8FF9957FD6B}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{A8859714-6683-404F-8B3E-C22B934A0402}"/>
-    <hyperlink ref="B9:B21" r:id="rId8" display="sdgsdg16@sdfs.com" xr:uid="{20AB0FA0-2FCF-4946-805C-1786454A6D88}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{63DE5FC5-7796-4B4B-81DD-D968321D9C6B}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{F913C886-98A3-41E6-BC5F-8B084A682B37}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{DB2A5EBF-0D1B-48AD-A028-6875EB1EC24C}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{AB0A9AB9-08C8-487E-BED6-CDA02C3BDD30}"/>
-    <hyperlink ref="B13" r:id="rId13" xr:uid="{0FB8CA00-5952-4E8C-8530-1B6409D59E58}"/>
-    <hyperlink ref="B14" r:id="rId14" xr:uid="{87AD1E5E-C3C8-42BE-8BFF-D9C37FB3BB49}"/>
-    <hyperlink ref="B15" r:id="rId15" xr:uid="{F16A30EB-5832-4AEB-8C48-00D882BCA876}"/>
-    <hyperlink ref="B16" r:id="rId16" xr:uid="{C775F62E-B4EF-4092-A98E-62299259C923}"/>
-    <hyperlink ref="B17" r:id="rId17" xr:uid="{5D33633F-C834-461B-A633-5E70164F146F}"/>
-    <hyperlink ref="B18" r:id="rId18" xr:uid="{CDE686AB-472F-40A3-A751-F3DE31BC1925}"/>
-    <hyperlink ref="B19" r:id="rId19" xr:uid="{6BE61DC1-AE4E-4A8F-8B8F-2E08F8452C9C}"/>
-    <hyperlink ref="B20" r:id="rId20" xr:uid="{2CC438B5-3777-4FF2-9FC6-B490BF887D25}"/>
-    <hyperlink ref="B21" r:id="rId21" xr:uid="{D95EC583-2414-4D23-8E3A-00730D40F27E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A505EBCF-EC70-40E4-9280-A9DC40CD467D}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1789,7 +1560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65954F3C-4D75-4AB4-A83A-42172BC3382B}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -2110,4 +1881,525 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4973ED3-E61C-42D5-8CE6-08AD080CDC15}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{EC05753F-FE94-4927-9DB7-10585008DC02}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{31DC19B5-7C5C-43F9-ABB1-92E11E055F29}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{3F406CCA-DE58-41E3-BFBD-D92467B62273}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{148DA2B8-9DA5-4116-8A7A-73DBFDDF7707}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{7D3B08B7-95EE-4AB4-9828-6FE63C4B2901}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{E88D3398-B6E6-4845-9FD6-F8FF9957FD6B}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{A8859714-6683-404F-8B3E-C22B934A0402}"/>
+    <hyperlink ref="B9:B21" r:id="rId8" display="sdgsdg16@sdfs.com" xr:uid="{20AB0FA0-2FCF-4946-805C-1786454A6D88}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{63DE5FC5-7796-4B4B-81DD-D968321D9C6B}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{F913C886-98A3-41E6-BC5F-8B084A682B37}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{DB2A5EBF-0D1B-48AD-A028-6875EB1EC24C}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{AB0A9AB9-08C8-487E-BED6-CDA02C3BDD30}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{0FB8CA00-5952-4E8C-8530-1B6409D59E58}"/>
+    <hyperlink ref="B14" r:id="rId14" xr:uid="{87AD1E5E-C3C8-42BE-8BFF-D9C37FB3BB49}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{F16A30EB-5832-4AEB-8C48-00D882BCA876}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{C775F62E-B4EF-4092-A98E-62299259C923}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{5D33633F-C834-461B-A633-5E70164F146F}"/>
+    <hyperlink ref="B18" r:id="rId18" xr:uid="{CDE686AB-472F-40A3-A751-F3DE31BC1925}"/>
+    <hyperlink ref="B19" r:id="rId19" xr:uid="{6BE61DC1-AE4E-4A8F-8B8F-2E08F8452C9C}"/>
+    <hyperlink ref="B20" r:id="rId20" xr:uid="{2CC438B5-3777-4FF2-9FC6-B490BF887D25}"/>
+    <hyperlink ref="B21" r:id="rId21" xr:uid="{D95EC583-2414-4D23-8E3A-00730D40F27E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E656F44-F0E2-4355-A222-0001DFF6271C}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" customWidth="1"/>
+    <col min="23" max="23" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>190</v>
+      </c>
+      <c r="R1" t="s">
+        <v>191</v>
+      </c>
+      <c r="S1" t="s">
+        <v>192</v>
+      </c>
+      <c r="T1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V1" t="s">
+        <v>195</v>
+      </c>
+      <c r="W1" t="s">
+        <v>196</v>
+      </c>
+      <c r="X1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2">
+        <v>90909090909090</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2">
+        <v>282001</v>
+      </c>
+      <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" t="s">
+        <v>205</v>
+      </c>
+      <c r="K2">
+        <v>9090909090</v>
+      </c>
+      <c r="L2" s="2">
+        <v>36078</v>
+      </c>
+      <c r="M2" t="s">
+        <v>204</v>
+      </c>
+      <c r="N2" t="s">
+        <v>203</v>
+      </c>
+      <c r="O2" t="s">
+        <v>202</v>
+      </c>
+      <c r="P2" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>200</v>
+      </c>
+      <c r="R2" t="s">
+        <v>200</v>
+      </c>
+      <c r="S2" t="s">
+        <v>200</v>
+      </c>
+      <c r="T2" t="s">
+        <v>200</v>
+      </c>
+      <c r="U2" t="s">
+        <v>200</v>
+      </c>
+      <c r="V2" t="s">
+        <v>200</v>
+      </c>
+      <c r="W2" t="s">
+        <v>199</v>
+      </c>
+      <c r="X2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{9D2BE821-7B88-4799-8B13-0D867A7D35A8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
dob added in test cases
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Scripts for Testing\maven-testng\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam.kumar\Desktop\testCasesOfcaseStudy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2557A4B-CFDE-4852-BBA6-9F6D52462A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C189498-A5F2-480A-B3BD-B7D4AF6DE84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="217">
   <si>
     <t xml:space="preserve">shivam </t>
   </si>
@@ -650,6 +650,36 @@
   </si>
   <si>
     <t>Agra</t>
+  </si>
+  <si>
+    <t>2000-01-01</t>
+  </si>
+  <si>
+    <t>2000-01-02</t>
+  </si>
+  <si>
+    <t>2000-01-03</t>
+  </si>
+  <si>
+    <t>2000-01-04</t>
+  </si>
+  <si>
+    <t>2000-01-05</t>
+  </si>
+  <si>
+    <t>2000-01-06</t>
+  </si>
+  <si>
+    <t>2000-01-07</t>
+  </si>
+  <si>
+    <t>2000-01-08</t>
+  </si>
+  <si>
+    <t>2000-01-09</t>
+  </si>
+  <si>
+    <t>2000-01-10</t>
   </si>
 </sst>
 </file>
@@ -700,11 +730,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -986,355 +1017,422 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="2" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="sdvsdv@sdfds.com" xr:uid="{EE755B02-7380-4A9B-B5EE-CB261AF69109}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{28FC4BFD-C9B9-4A35-9B96-DE41AF25005A}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{5D582B9D-703D-4B9B-A0FD-635338541F92}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{28F54B58-3B3C-4E29-9C28-CD8518249D78}"/>
-    <hyperlink ref="C5:C16" r:id="rId5" display="sdfsf@sdfsg.com" xr:uid="{2286C9E7-4E8F-4B5B-8E82-2D9395FE000F}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{956C778D-F7DD-4AD2-9F3A-8E21AA6EDCFC}"/>
-    <hyperlink ref="C6" r:id="rId7" xr:uid="{7FA18995-56B2-4CE9-ACEC-C917D2D30DDB}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{4EE99F4C-5DD0-4734-A01B-4D1659EF225C}"/>
-    <hyperlink ref="C8" r:id="rId9" xr:uid="{89C3755F-7AB7-447A-AEA5-9DAAA5BBCBF9}"/>
-    <hyperlink ref="C9" r:id="rId10" xr:uid="{4A0C3F81-CC1F-4F36-8D7C-FEDEFF022ADA}"/>
-    <hyperlink ref="C10" r:id="rId11" xr:uid="{C39C3282-46DE-4B80-9265-558A7818C1EA}"/>
-    <hyperlink ref="C11" r:id="rId12" xr:uid="{FD01D7B3-678E-4B91-A997-954DB8575B48}"/>
-    <hyperlink ref="C12" r:id="rId13" xr:uid="{1ECBE6E4-EEA7-4A82-B712-8EC61566F097}"/>
-    <hyperlink ref="C13" r:id="rId14" xr:uid="{5AF9988B-E79E-491A-A242-482B39621D50}"/>
-    <hyperlink ref="C14" r:id="rId15" xr:uid="{57C50869-3736-4824-8331-62BA6083EA85}"/>
-    <hyperlink ref="C15" r:id="rId16" xr:uid="{F4797CFF-55BE-4590-A5D2-8DCE37534960}"/>
-    <hyperlink ref="C16" r:id="rId17" xr:uid="{1AAD59A6-5EFB-4EE1-859B-CD74E916F45B}"/>
-    <hyperlink ref="C17" r:id="rId18" xr:uid="{E55D8C2C-1B59-4D4E-8382-F6E24E36A9BE}"/>
-    <hyperlink ref="C18:C21" r:id="rId19" display="uttamkumarsingh@gmail.com" xr:uid="{B8E64D4F-53DA-426A-B6B3-649DEB8ED7CC}"/>
-    <hyperlink ref="C18" r:id="rId20" xr:uid="{B483E33E-D31F-436E-A6EA-134A72F46DA7}"/>
-    <hyperlink ref="C19" r:id="rId21" xr:uid="{4B10FBF8-DABB-49D8-819A-9CFFA16C512F}"/>
-    <hyperlink ref="C20" r:id="rId22" xr:uid="{44FD0A7B-1AB2-4B9D-80C6-D2449BBAF32D}"/>
-    <hyperlink ref="C21" r:id="rId23" xr:uid="{ABF9DFC1-FDD1-426C-A595-D690BE24B855}"/>
-    <hyperlink ref="C22" r:id="rId24" xr:uid="{42279FB4-4D6C-4BA4-8020-115869F10136}"/>
+    <hyperlink ref="D1" r:id="rId1" display="sdvsdv@sdfds.com" xr:uid="{EE755B02-7380-4A9B-B5EE-CB261AF69109}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{28FC4BFD-C9B9-4A35-9B96-DE41AF25005A}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{5D582B9D-703D-4B9B-A0FD-635338541F92}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{28F54B58-3B3C-4E29-9C28-CD8518249D78}"/>
+    <hyperlink ref="D5:D16" r:id="rId5" display="sdfsf@sdfsg.com" xr:uid="{2286C9E7-4E8F-4B5B-8E82-2D9395FE000F}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{956C778D-F7DD-4AD2-9F3A-8E21AA6EDCFC}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{7FA18995-56B2-4CE9-ACEC-C917D2D30DDB}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{4EE99F4C-5DD0-4734-A01B-4D1659EF225C}"/>
+    <hyperlink ref="D8" r:id="rId9" xr:uid="{89C3755F-7AB7-447A-AEA5-9DAAA5BBCBF9}"/>
+    <hyperlink ref="D9" r:id="rId10" xr:uid="{4A0C3F81-CC1F-4F36-8D7C-FEDEFF022ADA}"/>
+    <hyperlink ref="D10" r:id="rId11" xr:uid="{C39C3282-46DE-4B80-9265-558A7818C1EA}"/>
+    <hyperlink ref="D11" r:id="rId12" xr:uid="{FD01D7B3-678E-4B91-A997-954DB8575B48}"/>
+    <hyperlink ref="D12" r:id="rId13" xr:uid="{1ECBE6E4-EEA7-4A82-B712-8EC61566F097}"/>
+    <hyperlink ref="D13" r:id="rId14" xr:uid="{5AF9988B-E79E-491A-A242-482B39621D50}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{57C50869-3736-4824-8331-62BA6083EA85}"/>
+    <hyperlink ref="D15" r:id="rId16" xr:uid="{F4797CFF-55BE-4590-A5D2-8DCE37534960}"/>
+    <hyperlink ref="D16" r:id="rId17" xr:uid="{1AAD59A6-5EFB-4EE1-859B-CD74E916F45B}"/>
+    <hyperlink ref="D17" r:id="rId18" xr:uid="{E55D8C2C-1B59-4D4E-8382-F6E24E36A9BE}"/>
+    <hyperlink ref="D18:D21" r:id="rId19" display="uttamkumarsingh@gmail.com" xr:uid="{B8E64D4F-53DA-426A-B6B3-649DEB8ED7CC}"/>
+    <hyperlink ref="D18" r:id="rId20" xr:uid="{B483E33E-D31F-436E-A6EA-134A72F46DA7}"/>
+    <hyperlink ref="D19" r:id="rId21" xr:uid="{4B10FBF8-DABB-49D8-819A-9CFFA16C512F}"/>
+    <hyperlink ref="D20" r:id="rId22" xr:uid="{44FD0A7B-1AB2-4B9D-80C6-D2449BBAF32D}"/>
+    <hyperlink ref="D21" r:id="rId23" xr:uid="{ABF9DFC1-FDD1-426C-A595-D690BE24B855}"/>
+    <hyperlink ref="D22" r:id="rId24" xr:uid="{42279FB4-4D6C-4BA4-8020-115869F10136}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -2227,7 +2325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E656F44-F0E2-4355-A222-0001DFF6271C}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>